<commit_message>
SQL + Pandas mini-course
</commit_message>
<xml_diff>
--- a/Excel/Books-Findings.xlsx
+++ b/Excel/Books-Findings.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fede Cocimano\Documents\ROAD-TO-DATA-CAREER\StarkIndustries-SpecialProjects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BA8A01-D185-4DF0-BD97-50AD95F21569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D632BB9-1F5E-48F4-954B-7E2ECF6807B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books-Clean" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Books-Clean'!$A$1:$F$171</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="567">
   <si>
     <t>Book</t>
   </si>
@@ -1750,6 +1749,15 @@
   </si>
   <si>
     <t>Dystopian Fiction</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Approximate sales</t>
   </si>
 </sst>
 </file>
@@ -2892,7 +2900,178 @@
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Book" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="170">
+        <s v="A Tale of Two Cities"/>
+        <s v="The Little Prince"/>
+        <s v="Harry Potter and the Philosopher's Stone"/>
+        <s v="And Then There Were None"/>
+        <s v="Dream of the Red Chamber"/>
+        <s v="The Hobbit"/>
+        <s v="She: A History of Adventure"/>
+        <s v="Vardi Wala Gunda"/>
+        <s v="The Da Vinci Code"/>
+        <s v="Harry Potter and the Chamber of Secrets"/>
+        <s v="Harry Potter and the Prisoner of Azkaban"/>
+        <s v="Harry Potter and the Goblet of Fire"/>
+        <s v="Harry Potter and the Order of the Phoenix"/>
+        <s v="Harry Potter and the Half-Blood Prince"/>
+        <s v="Harry Potter and the Deathly Hallows"/>
+        <s v="The Alchemist"/>
+        <s v="The Catcher in the Rye"/>
+        <s v="The Bridges of Madison County"/>
+        <s v="One Hundred Years of Solitude"/>
+        <s v="Lolita"/>
+        <s v="Heidi"/>
+        <s v="The Common Sense Book of Baby and Child Care"/>
+        <s v="Anne of Green Gables"/>
+        <s v="Black Beauty"/>
+        <s v="The Name of the Rose"/>
+        <s v="The Eagle Has Landed"/>
+        <s v="Watership Down"/>
+        <s v="The Hite Report"/>
+        <s v="Charlotte's Web"/>
+        <s v="The Ginger Man"/>
+        <s v="Where the Crawdads Sing"/>
+        <s v="Matilda"/>
+        <s v="The Book Thief"/>
+        <s v="The Horse Whisperer"/>
+        <s v="Goodnight Moon"/>
+        <s v="The Neverending Story"/>
+        <s v="All the Light We Cannot See"/>
+        <s v="Fifty Shades of Grey"/>
+        <s v="The Outsiders"/>
+        <s v="Guess How Much I Love You"/>
+        <s v="Sh?gun"/>
+        <s v="The Poky Little Puppy"/>
+        <s v="The Pillars of the Earth"/>
+        <s v="Perfume"/>
+        <s v="The Grapes of Wrath"/>
+        <s v="The Shadow of the Wind"/>
+        <s v="Interpreter of Maladies"/>
+        <s v="Becoming"/>
+        <s v="The Hitchhiker's Guide to the Galaxy"/>
+        <s v="Tuesdays with Morrie"/>
+        <s v="God's Little Acre"/>
+        <s v="Follow Your Heart"/>
+        <s v="A Wrinkle in Time"/>
+        <s v="Long Walk to Freedom"/>
+        <s v="The Old Man and the Sea"/>
+        <s v="Life After Life"/>
+        <s v="The Tale of Peter Rabbit"/>
+        <s v="Jonathan Livingston Seagull"/>
+        <s v="The Very Hungry Caterpillar"/>
+        <s v="A Message to Garcia"/>
+        <s v="To Kill a Mockingbird"/>
+        <s v="Flowers in the Attic"/>
+        <s v="Cosmos"/>
+        <s v="Sophie's World"/>
+        <s v="Angels &amp; Demons"/>
+        <s v="Kane and Abel"/>
+        <s v="How the Steel Was Tempered"/>
+        <s v="War and Peace"/>
+        <s v="The Adventures of Pinocchio"/>
+        <s v="The Diary of Anne Frank"/>
+        <s v="Your Erroneous Zones"/>
+        <s v="The Thorn Birds"/>
+        <s v="The Kite Runner"/>
+        <s v="Valley of the Dolls"/>
+        <s v="How to Win Friends and Influence People"/>
+        <s v="The Great Gatsby"/>
+        <s v="Gone with the Wind"/>
+        <s v="Rebecca"/>
+        <s v="The Revolt of Mamie Stover"/>
+        <s v="The Girl with the Dragon Tattoo"/>
+        <s v="The Lost Symbol"/>
+        <s v="The Hunger Games"/>
+        <s v="James and the Giant Peach"/>
+        <s v="The Young Guard"/>
+        <s v="Who Moved My Cheese?"/>
+        <s v="A Brief History of Time"/>
+        <s v="Paul et Virginie"/>
+        <s v="Lust for Life"/>
+        <s v="The Wind in the Willows"/>
+        <s v="The 7 Habits of Highly Effective People"/>
+        <s v="Totto-Chan: The Little Girl at the Window"/>
+        <s v="Virgin Soil Upturned"/>
+        <s v="The Celestine Prophecy"/>
+        <s v="The Fault in Our Stars"/>
+        <s v="The Girl on the Train"/>
+        <s v="The Shack"/>
+        <s v="Uncle Styopa"/>
+        <s v="The Godfather"/>
+        <s v="Love Story"/>
+        <s v="Catching Fire"/>
+        <s v="Mockingjay"/>
+        <s v="Kitchen"/>
+        <s v="Andromeda Nebula"/>
+        <s v="Gone Girl"/>
+        <s v="The Bermuda Triangle"/>
+        <s v="Things Fall Apart"/>
+        <s v="Wolf Totem"/>
+        <s v="The Happy Hooker: My Own Story"/>
+        <s v="Jaws"/>
+        <s v="Love You Forever"/>
+        <s v="The Women's Room"/>
+        <s v="What to Expect When You're Expecting"/>
+        <s v="Adventures of Huckleberry Finn"/>
+        <s v="The Secret Diary of Adrian Mole, Aged 13¾"/>
+        <s v="Pride and Prejudice"/>
+        <s v="Kon-Tiki: Across the Pacific in a Raft"/>
+        <s v="The Good Soldier vejk"/>
+        <s v="Where the Wild Things Are"/>
+        <s v="The Power of Positive Thinking"/>
+        <s v="The Secret"/>
+        <s v="Fear of Flying"/>
+        <s v="Dune"/>
+        <s v="Charlie and the Chocolate Factory"/>
+        <s v="The Naked Ape"/>
+        <s v="Momo"/>
+        <s v="Peyton Place"/>
+        <s v="The Giver"/>
+        <s v="Me Before You"/>
+        <s v="Norwegian Wood"/>
+        <s v="The Plague"/>
+        <s v="No Longer Human"/>
+        <s v="Man's Search for Meaning"/>
+        <s v="The Divine Comedy"/>
+        <s v="The Prophet"/>
+        <s v="The Boy in the Striped Pyjamas"/>
+        <s v="The Exorcist"/>
+        <s v="The Gruffalo"/>
+        <s v="Fifty Shades Darker"/>
+        <s v="Tobacco Road"/>
+        <s v="Ronia, the Robber's Daughter"/>
+        <s v="The Cat in the Hat"/>
+        <s v="Diana: Her True Story"/>
+        <s v="The Help"/>
+        <s v="Catch-22"/>
+        <s v="The Stranger"/>
+        <s v="Eye of the Needle"/>
+        <s v="The Lovely Bones"/>
+        <s v="Wild Swans"/>
+        <s v="Santa Evita"/>
+        <s v="Night"/>
+        <s v="Confucius from the Heart"/>
+        <s v="The Total Woman"/>
+        <s v="Knowledge-value Revolution"/>
+        <s v="Problems in China's Socialist Economy"/>
+        <s v="What Color Is Your Parachute?"/>
+        <s v="The Dukan Diet"/>
+        <s v="The Joy of Sex"/>
+        <s v="The Gospel According to Peanuts"/>
+        <s v="The Subtle Art of Not Giving a Fuck"/>
+        <s v="Life of Pi"/>
+        <s v="The Front Runner"/>
+        <s v="The Goal"/>
+        <s v="Fahrenheit 451"/>
+        <s v="Angela's Ashes"/>
+        <s v="The Story of My Experiments with Truth"/>
+        <s v="Bridget Jones's Diary"/>
+        <s v="World Almanac"/>
+        <s v="Betty Crocker Cookbook"/>
+        <s v="Tung Shing"/>
+        <s v="Merriam-Webster's Collegiate Dictionary"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Author(s)" numFmtId="0">
       <sharedItems/>
@@ -2921,7 +3100,61 @@
       <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1868" maxValue="1996"/>
     </cacheField>
     <cacheField name="Approximate sales" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="53">
+        <s v="&gt;200 million"/>
+        <s v="200 million"/>
+        <s v="120 million"/>
+        <s v="100 million"/>
+        <s v="83 million"/>
+        <s v="&gt;80 million"/>
+        <s v="80 million"/>
+        <s v="77 million"/>
+        <s v="65 million"/>
+        <s v="60 million"/>
+        <s v="50 million"/>
+        <s v="18 million"/>
+        <s v="17 million"/>
+        <s v="16 million"/>
+        <s v="15.3 million"/>
+        <s v="15.2 million"/>
+        <s v="15 million"/>
+        <s v="14 million"/>
+        <s v="13 million"/>
+        <s v="45 million"/>
+        <s v="44 million"/>
+        <s v="43 million"/>
+        <s v="40 million"/>
+        <s v="39 million"/>
+        <s v="37 million"/>
+        <s v="36.4 million"/>
+        <s v="36 million"/>
+        <s v="35 million"/>
+        <s v="33 million"/>
+        <s v="31.5 million"/>
+        <s v="31 million"/>
+        <s v="&gt;30 million"/>
+        <s v="30 million"/>
+        <s v="29 million"/>
+        <s v="28 million"/>
+        <s v="26 million"/>
+        <s v="25 million"/>
+        <s v="24 million"/>
+        <s v="23 million"/>
+        <s v="22.5 million"/>
+        <s v="21 million"/>
+        <s v="20 million"/>
+        <s v="12.1 million"/>
+        <s v="12 million"/>
+        <s v="1112 million"/>
+        <s v="11 million"/>
+        <s v="10.5 million"/>
+        <s v="10.4 million"/>
+        <s v="10 million"/>
+        <s v="82 million"/>
+        <s v="75 million"/>
+        <s v="&gt;70 million"/>
+        <s v="55 million"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Genre" numFmtId="0">
       <sharedItems count="72">
@@ -3011,1370 +3244,2148 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="170">
   <r>
-    <s v="A Tale of Two Cities"/>
+    <x v="0"/>
     <s v="Charles Dickens"/>
     <x v="0"/>
     <s v="1859"/>
-    <s v="&gt;200 million"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="The Little Prince"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
     <s v="Antoine de Saint-Exupéry"/>
     <x v="1"/>
     <s v="1943"/>
-    <s v="200 million"/>
     <x v="1"/>
-  </r>
-  <r>
-    <s v="Harry Potter and the Philosopher's Stone"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
     <s v="J. K. Rowling"/>
     <x v="0"/>
     <s v="1997"/>
-    <s v="120 million"/>
+    <x v="2"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="And Then There Were None"/>
+    <x v="3"/>
     <s v="Agatha Christie"/>
     <x v="0"/>
     <s v="1939"/>
-    <s v="100 million"/>
+    <x v="3"/>
     <x v="2"/>
   </r>
   <r>
-    <s v="Dream of the Red Chamber"/>
+    <x v="4"/>
     <s v="Cao Xueqin"/>
     <x v="2"/>
     <s v="1791"/>
-    <s v="100 million"/>
     <x v="3"/>
-  </r>
-  <r>
-    <s v="The Hobbit"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="5"/>
     <s v="J. R. R. Tolkien"/>
     <x v="0"/>
     <s v="1937"/>
-    <s v="100 million"/>
+    <x v="3"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="She: A History of Adventure"/>
+    <x v="6"/>
     <s v="H. Rider Haggard"/>
     <x v="0"/>
     <s v="1887"/>
-    <s v="83 million"/>
     <x v="4"/>
-  </r>
-  <r>
-    <s v="Vardi Wala Gunda"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="7"/>
     <s v="Ved Prakash Sharma"/>
     <x v="3"/>
     <s v="1992"/>
-    <s v="&gt;80 million"/>
     <x v="5"/>
-  </r>
-  <r>
-    <s v="The Da Vinci Code"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="8"/>
     <s v="Dan Brown"/>
     <x v="0"/>
     <s v="2003"/>
-    <s v="80 million"/>
     <x v="6"/>
-  </r>
-  <r>
-    <s v="Harry Potter and the Chamber of Secrets"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="9"/>
     <s v="J. K. Rowling"/>
     <x v="0"/>
     <s v="1998"/>
-    <s v="77 million"/>
     <x v="7"/>
-  </r>
-  <r>
-    <s v="Harry Potter and the Prisoner of Azkaban"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="10"/>
     <s v="J. K. Rowling"/>
     <x v="0"/>
     <s v="1999"/>
-    <s v="65 million"/>
+    <x v="8"/>
     <x v="7"/>
   </r>
   <r>
-    <s v="Harry Potter and the Goblet of Fire"/>
+    <x v="11"/>
     <s v="J. K. Rowling"/>
     <x v="0"/>
     <s v="2000"/>
-    <s v="65 million"/>
+    <x v="8"/>
     <x v="7"/>
   </r>
   <r>
-    <s v="Harry Potter and the Order of the Phoenix"/>
+    <x v="12"/>
     <s v="J. K. Rowling"/>
     <x v="0"/>
     <s v="2003"/>
-    <s v="65 million"/>
+    <x v="8"/>
     <x v="7"/>
   </r>
   <r>
-    <s v="Harry Potter and the Half-Blood Prince"/>
+    <x v="13"/>
     <s v="J. K. Rowling"/>
     <x v="0"/>
     <s v="2005"/>
-    <s v="65 million"/>
+    <x v="8"/>
     <x v="7"/>
   </r>
   <r>
-    <s v="Harry Potter and the Deathly Hallows"/>
+    <x v="14"/>
     <s v="J. K. Rowling"/>
     <x v="0"/>
     <s v="2007"/>
-    <s v="65 million"/>
+    <x v="8"/>
     <x v="7"/>
   </r>
   <r>
-    <s v="The Alchemist"/>
+    <x v="15"/>
     <s v="Paulo Coelho"/>
     <x v="4"/>
     <s v="1988"/>
-    <s v="65 million"/>
+    <x v="8"/>
     <x v="7"/>
   </r>
   <r>
-    <s v="The Catcher in the Rye"/>
+    <x v="16"/>
     <s v="J. D. Salinger"/>
     <x v="0"/>
     <s v="1951"/>
-    <s v="65 million"/>
     <x v="8"/>
-  </r>
-  <r>
-    <s v="The Bridges of Madison County"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="17"/>
     <s v="Robert James Waller"/>
     <x v="0"/>
     <s v="1992"/>
-    <s v="60 million"/>
     <x v="9"/>
-  </r>
-  <r>
-    <s v="One Hundred Years of Solitude"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="18"/>
     <s v="Gabriel García Márquez"/>
     <x v="5"/>
     <s v="1967"/>
-    <s v="50 million"/>
     <x v="10"/>
-  </r>
-  <r>
-    <s v="Lolita"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="19"/>
     <s v="Vladimir Nabokov"/>
     <x v="0"/>
     <s v="1955"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="11"/>
   </r>
   <r>
-    <s v="Heidi"/>
+    <x v="20"/>
     <s v="Johanna Spyri"/>
     <x v="6"/>
     <s v="1880"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="12"/>
   </r>
   <r>
-    <s v="The Common Sense Book of Baby and Child Care"/>
+    <x v="21"/>
     <s v="Benjamin Spock"/>
     <x v="0"/>
     <s v="1946"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="13"/>
   </r>
   <r>
-    <s v="Anne of Green Gables"/>
+    <x v="22"/>
     <s v="Lucy Maud Montgomery"/>
     <x v="0"/>
     <s v="1908"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="14"/>
   </r>
   <r>
-    <s v="Black Beauty"/>
+    <x v="23"/>
     <s v="Anna Sewell"/>
     <x v="0"/>
     <s v="1877"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="15"/>
   </r>
   <r>
-    <s v="The Name of the Rose"/>
+    <x v="24"/>
     <s v="Umberto Eco"/>
     <x v="7"/>
     <s v="1980"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="16"/>
   </r>
   <r>
-    <s v="The Eagle Has Landed"/>
+    <x v="25"/>
     <s v="Jack Higgins"/>
     <x v="0"/>
     <s v="1975"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="17"/>
   </r>
   <r>
-    <s v="Watership Down"/>
+    <x v="26"/>
     <s v="Richard Adams"/>
     <x v="0"/>
     <s v="1972"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="7"/>
   </r>
   <r>
-    <s v="The Hite Report"/>
+    <x v="27"/>
     <s v="Shere Hite"/>
     <x v="0"/>
     <s v="1976"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="18"/>
   </r>
   <r>
-    <s v="Charlotte's Web"/>
+    <x v="28"/>
     <s v="E. B. White; illustrated by Garth Williams"/>
     <x v="0"/>
     <s v="1952"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="12"/>
   </r>
   <r>
-    <s v="The Ginger Man"/>
+    <x v="29"/>
     <s v="J. P. Donleavy"/>
     <x v="0"/>
     <s v="1955"/>
-    <s v="50 million"/>
+    <x v="10"/>
     <x v="11"/>
   </r>
   <r>
-    <s v="Where the Crawdads Sing"/>
+    <x v="30"/>
     <s v="Delia Owens"/>
     <x v="0"/>
     <s v="2018"/>
-    <s v="18 million"/>
+    <x v="11"/>
     <x v="19"/>
   </r>
   <r>
-    <s v="Matilda"/>
+    <x v="31"/>
     <s v="Roald Dahl"/>
     <x v="0"/>
     <s v="1988"/>
-    <s v="17 million"/>
+    <x v="12"/>
     <x v="15"/>
   </r>
   <r>
-    <s v="The Book Thief"/>
+    <x v="32"/>
     <s v="Markus Zusak"/>
     <x v="0"/>
     <s v="2005"/>
-    <s v="16 million"/>
+    <x v="13"/>
     <x v="20"/>
   </r>
   <r>
-    <s v="The Horse Whisperer"/>
+    <x v="33"/>
     <s v="Nicholas Evans"/>
     <x v="0"/>
     <s v="1995"/>
-    <s v="16 million"/>
+    <x v="13"/>
     <x v="20"/>
   </r>
   <r>
-    <s v="Goodnight Moon"/>
+    <x v="34"/>
     <s v="Margaret Wise Brown"/>
     <x v="0"/>
     <s v="1947"/>
-    <s v="16 million"/>
+    <x v="13"/>
     <x v="15"/>
   </r>
   <r>
-    <s v="The Neverending Story"/>
+    <x v="35"/>
     <s v="Michael Ende"/>
     <x v="6"/>
     <s v="1979"/>
-    <s v="16 million"/>
+    <x v="13"/>
     <x v="15"/>
   </r>
   <r>
-    <s v="All the Light We Cannot See"/>
+    <x v="36"/>
     <s v="Anthony Doerr"/>
     <x v="0"/>
     <s v="2014"/>
-    <s v="15.3 million"/>
+    <x v="14"/>
     <x v="21"/>
   </r>
   <r>
-    <s v="Fifty Shades of Grey"/>
+    <x v="37"/>
     <s v="E. L. James"/>
     <x v="0"/>
     <s v="2011"/>
-    <s v="15.2 million"/>
+    <x v="15"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Outsiders"/>
+    <x v="38"/>
     <s v="S. E. Hinton"/>
     <x v="0"/>
     <s v="1967"/>
-    <s v="15 million"/>
+    <x v="16"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Guess How Much I Love You"/>
+    <x v="39"/>
     <s v="Sam McBratney"/>
     <x v="0"/>
     <s v="1994"/>
-    <s v="15 million"/>
+    <x v="16"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Sh?gun"/>
+    <x v="40"/>
     <s v="James Clavell"/>
     <x v="0"/>
     <s v="1975"/>
-    <s v="15 million"/>
+    <x v="16"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Poky Little Puppy"/>
+    <x v="41"/>
     <s v="Janette Sebring Lowrey"/>
     <x v="0"/>
     <s v="1942"/>
-    <s v="15 million"/>
+    <x v="16"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Pillars of the Earth"/>
+    <x v="42"/>
     <s v="Ken Follett"/>
     <x v="0"/>
     <s v="1989"/>
-    <s v="15 million"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Perfume"/>
+    <x v="16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="43"/>
     <s v="Patrick Süskind"/>
     <x v="6"/>
     <s v="1985"/>
-    <s v="15 million"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="The Grapes of Wrath"/>
+    <x v="16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="44"/>
     <s v="John Steinbeck"/>
     <x v="0"/>
     <s v="1939"/>
-    <s v="15 million"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="The Shadow of the Wind"/>
+    <x v="16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="45"/>
     <s v="Carlos Ruiz Zafón"/>
     <x v="5"/>
     <s v="2001"/>
-    <s v="15 million"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Interpreter of Maladies"/>
+    <x v="16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="46"/>
     <s v="Jhumpa Lahiri"/>
     <x v="0"/>
     <s v="2000"/>
-    <s v="15 million"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Becoming"/>
+    <x v="16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="47"/>
     <s v="Michelle Obama"/>
     <x v="0"/>
     <s v="2018"/>
-    <s v="14 million"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="The Hitchhiker's Guide to the Galaxy"/>
+    <x v="17"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="48"/>
     <s v="Douglas Adams"/>
     <x v="0"/>
     <s v="1979"/>
-    <s v="14 million"/>
+    <x v="17"/>
     <x v="23"/>
   </r>
   <r>
-    <s v="Tuesdays with Morrie"/>
+    <x v="49"/>
     <s v="Mitch Albom"/>
     <x v="0"/>
     <s v="1997"/>
-    <s v="14 million"/>
+    <x v="17"/>
     <x v="23"/>
   </r>
   <r>
-    <s v="God's Little Acre"/>
+    <x v="50"/>
     <s v="Erskine Caldwell"/>
     <x v="0"/>
     <s v="1933"/>
-    <s v="14 million"/>
+    <x v="17"/>
     <x v="23"/>
   </r>
   <r>
-    <s v="Follow Your Heart"/>
+    <x v="51"/>
     <s v="Susanna Tamaro"/>
     <x v="7"/>
     <s v="1994"/>
-    <s v="14 million"/>
+    <x v="17"/>
     <x v="23"/>
   </r>
   <r>
-    <s v="A Wrinkle in Time"/>
+    <x v="52"/>
     <s v="Madeleine L'Engle"/>
     <x v="0"/>
     <s v="1962"/>
-    <s v="14 million"/>
+    <x v="17"/>
     <x v="23"/>
   </r>
   <r>
-    <s v="Long Walk to Freedom"/>
+    <x v="53"/>
     <s v="Nelson Mandela"/>
     <x v="0"/>
     <s v="1994"/>
-    <s v="14 million"/>
+    <x v="17"/>
     <x v="23"/>
   </r>
   <r>
-    <s v="The Old Man and the Sea"/>
+    <x v="54"/>
     <s v="Ernest Hemingway"/>
     <x v="0"/>
     <s v="1952"/>
-    <s v="13 million"/>
+    <x v="18"/>
     <x v="23"/>
   </r>
   <r>
-    <s v="Life After Life"/>
+    <x v="55"/>
     <s v="Raymond Moody"/>
     <x v="0"/>
     <s v="1975"/>
-    <s v="13 million"/>
+    <x v="18"/>
     <x v="23"/>
   </r>
   <r>
-    <s v="The Tale of Peter Rabbit"/>
+    <x v="56"/>
     <s v="Beatrix Potter"/>
     <x v="0"/>
     <s v="1902"/>
-    <s v="45 million"/>
+    <x v="19"/>
     <x v="15"/>
   </r>
   <r>
-    <s v="Jonathan Livingston Seagull"/>
+    <x v="57"/>
     <s v="Richard Bach"/>
     <x v="0"/>
     <s v="1970"/>
-    <s v="44 million"/>
+    <x v="20"/>
     <x v="24"/>
   </r>
   <r>
-    <s v="The Very Hungry Caterpillar"/>
+    <x v="58"/>
     <s v="Eric Carle"/>
     <x v="0"/>
     <s v="1969"/>
-    <s v="43 million"/>
+    <x v="21"/>
     <x v="25"/>
   </r>
   <r>
-    <s v="A Message to Garcia"/>
+    <x v="59"/>
     <s v="Elbert Hubbard"/>
     <x v="0"/>
     <s v="1899"/>
-    <s v="40 million"/>
+    <x v="22"/>
     <x v="26"/>
   </r>
   <r>
-    <s v="To Kill a Mockingbird"/>
+    <x v="60"/>
     <s v="Harper Lee"/>
     <x v="0"/>
     <s v="1960"/>
-    <s v="40 million"/>
+    <x v="22"/>
     <x v="27"/>
   </r>
   <r>
-    <s v="Flowers in the Attic"/>
+    <x v="61"/>
     <s v="V. C. Andrews"/>
     <x v="0"/>
     <s v="1979"/>
-    <s v="40 million"/>
+    <x v="22"/>
     <x v="28"/>
   </r>
   <r>
-    <s v="Cosmos"/>
+    <x v="62"/>
     <s v="Carl Sagan"/>
     <x v="0"/>
     <s v="1980"/>
-    <s v="40 million"/>
+    <x v="22"/>
     <x v="29"/>
   </r>
   <r>
-    <s v="Sophie's World"/>
+    <x v="63"/>
     <s v="Jostein Gaarder"/>
     <x v="8"/>
     <s v="1991"/>
-    <s v="40 million"/>
+    <x v="22"/>
     <x v="30"/>
   </r>
   <r>
-    <s v="Angels &amp; Demons"/>
+    <x v="64"/>
     <s v="Dan Brown"/>
     <x v="0"/>
     <s v="2000"/>
-    <s v="39 million"/>
+    <x v="23"/>
     <x v="31"/>
   </r>
   <r>
-    <s v="Kane and Abel"/>
+    <x v="65"/>
     <s v="Jeffrey Archer"/>
     <x v="0"/>
     <s v="1979"/>
-    <s v="37 million"/>
+    <x v="24"/>
     <x v="11"/>
   </r>
   <r>
-    <s v="How the Steel Was Tempered"/>
+    <x v="66"/>
     <s v="Nikolai Ostrovsky"/>
     <x v="9"/>
     <s v="1932"/>
-    <s v="36.4 million"/>
+    <x v="25"/>
     <x v="32"/>
   </r>
   <r>
-    <s v="War and Peace"/>
+    <x v="67"/>
     <s v="Leo Tolstoy"/>
     <x v="9"/>
     <s v="1869"/>
-    <s v="36 million"/>
+    <x v="26"/>
     <x v="33"/>
   </r>
   <r>
-    <s v="The Adventures of Pinocchio"/>
+    <x v="68"/>
     <s v="Carlo Collodi"/>
     <x v="7"/>
     <s v="1881"/>
-    <s v="35 million"/>
+    <x v="27"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="The Diary of Anne Frank"/>
+    <x v="69"/>
     <s v="Anne Frank"/>
     <x v="10"/>
     <s v="1947"/>
-    <s v="35 million"/>
+    <x v="27"/>
     <x v="34"/>
   </r>
   <r>
-    <s v="Your Erroneous Zones"/>
+    <x v="70"/>
     <s v="Wayne Dyer"/>
     <x v="0"/>
     <s v="1976"/>
-    <s v="35 million"/>
+    <x v="27"/>
     <x v="35"/>
   </r>
   <r>
-    <s v="The Thorn Birds"/>
+    <x v="71"/>
     <s v="Colleen McCullough"/>
     <x v="0"/>
     <s v="1977"/>
-    <s v="33 million"/>
+    <x v="28"/>
     <x v="36"/>
   </r>
   <r>
-    <s v="The Kite Runner"/>
+    <x v="72"/>
     <s v="Khaled Hosseini"/>
     <x v="0"/>
     <s v="2003"/>
-    <s v="31.5 million"/>
+    <x v="29"/>
     <x v="37"/>
   </r>
   <r>
-    <s v="Valley of the Dolls"/>
+    <x v="73"/>
     <s v="Jacqueline Susann"/>
     <x v="0"/>
     <s v="1966"/>
-    <s v="31 million"/>
+    <x v="30"/>
     <x v="11"/>
   </r>
   <r>
-    <s v="How to Win Friends and Influence People"/>
+    <x v="74"/>
     <s v="Dale Carnegie"/>
     <x v="0"/>
     <s v="1936"/>
-    <s v="&gt;30 million"/>
+    <x v="31"/>
     <x v="35"/>
   </r>
   <r>
-    <s v="The Great Gatsby"/>
+    <x v="75"/>
     <s v="F. Scott Fitzgerald"/>
     <x v="0"/>
     <s v="1925"/>
-    <s v="30 million"/>
+    <x v="32"/>
     <x v="38"/>
   </r>
   <r>
-    <s v="Gone with the Wind"/>
+    <x v="76"/>
     <s v="Margaret Mitchell"/>
     <x v="0"/>
     <s v="1936"/>
-    <s v="30 million"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="Rebecca"/>
+    <x v="32"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="77"/>
     <s v="Daphne du Maurier"/>
     <x v="0"/>
     <s v="1938"/>
-    <s v="30 million"/>
+    <x v="32"/>
     <x v="39"/>
   </r>
   <r>
-    <s v="The Revolt of Mamie Stover"/>
+    <x v="78"/>
     <s v="William Bradford Huie"/>
     <x v="0"/>
     <s v="1951"/>
-    <s v="30 million"/>
+    <x v="32"/>
     <x v="40"/>
   </r>
   <r>
-    <s v="The Girl with the Dragon Tattoo"/>
+    <x v="79"/>
     <s v="Stieg Larsson"/>
     <x v="11"/>
     <s v="2005"/>
-    <s v="30 million"/>
+    <x v="32"/>
     <x v="40"/>
   </r>
   <r>
-    <s v="The Lost Symbol"/>
+    <x v="80"/>
     <s v="Dan Brown"/>
     <x v="0"/>
     <s v="2009"/>
-    <s v="30 million"/>
+    <x v="32"/>
     <x v="40"/>
   </r>
   <r>
-    <s v="The Hunger Games"/>
+    <x v="81"/>
     <s v="Suzanne Collins"/>
     <x v="0"/>
     <s v="2008"/>
-    <s v="29 million"/>
+    <x v="33"/>
     <x v="20"/>
   </r>
   <r>
-    <s v="James and the Giant Peach"/>
+    <x v="82"/>
     <s v="Roald Dahl"/>
     <x v="0"/>
     <s v="1961"/>
-    <s v="28 million"/>
+    <x v="34"/>
     <x v="14"/>
   </r>
   <r>
-    <s v="The Young Guard"/>
+    <x v="83"/>
     <s v="Alexander Alexandrovich Fadeyev"/>
     <x v="9"/>
     <s v="1945"/>
-    <s v="26 million"/>
+    <x v="35"/>
     <x v="41"/>
   </r>
   <r>
-    <s v="Who Moved My Cheese?"/>
+    <x v="84"/>
     <s v="Spencer Johnson"/>
     <x v="0"/>
     <s v="1998"/>
-    <s v="30 million"/>
+    <x v="32"/>
     <x v="42"/>
   </r>
   <r>
-    <s v="A Brief History of Time"/>
+    <x v="85"/>
     <s v="Stephen Hawking"/>
     <x v="0"/>
     <s v="1988"/>
-    <s v="25 million"/>
+    <x v="36"/>
     <x v="43"/>
   </r>
   <r>
-    <s v="Paul et Virginie"/>
+    <x v="86"/>
     <s v="Jacques-Henri Bernardin de Saint-Pierre"/>
     <x v="1"/>
     <s v="1788"/>
-    <s v="25 million"/>
+    <x v="36"/>
     <x v="11"/>
   </r>
   <r>
-    <s v="Lust for Life"/>
+    <x v="87"/>
     <s v="Irving Stone"/>
     <x v="0"/>
     <s v="1934"/>
-    <s v="25 million"/>
+    <x v="36"/>
     <x v="44"/>
   </r>
   <r>
-    <s v="The Wind in the Willows"/>
+    <x v="88"/>
     <s v="Kenneth Grahame"/>
     <x v="0"/>
     <s v="1908"/>
-    <s v="25 million"/>
+    <x v="36"/>
     <x v="15"/>
   </r>
   <r>
-    <s v="The 7 Habits of Highly Effective People"/>
+    <x v="89"/>
     <s v="Stephen R. Covey"/>
     <x v="0"/>
     <s v="1989"/>
-    <s v="25 million"/>
+    <x v="36"/>
     <x v="35"/>
   </r>
   <r>
-    <s v="Totto-Chan: The Little Girl at the Window"/>
+    <x v="90"/>
     <s v="Tetsuko Kuroyanagi"/>
     <x v="12"/>
     <s v="1981"/>
-    <s v="25 million"/>
+    <x v="36"/>
     <x v="45"/>
   </r>
   <r>
-    <s v="Virgin Soil Upturned"/>
+    <x v="91"/>
     <s v="Mikhail Sholokhov"/>
     <x v="9"/>
     <s v="1935"/>
-    <s v="24 million"/>
+    <x v="37"/>
     <x v="11"/>
   </r>
   <r>
-    <s v="The Celestine Prophecy"/>
+    <x v="92"/>
     <s v="James Redfield"/>
     <x v="0"/>
     <s v="1993"/>
-    <s v="23 million"/>
+    <x v="38"/>
     <x v="46"/>
   </r>
   <r>
-    <s v="The Fault in Our Stars"/>
+    <x v="93"/>
     <s v="John Green"/>
     <x v="0"/>
     <s v="2012"/>
-    <s v="23 million"/>
+    <x v="38"/>
     <x v="47"/>
   </r>
   <r>
-    <s v="The Girl on the Train"/>
+    <x v="94"/>
     <s v="Paula Hawkins"/>
     <x v="0"/>
     <s v="2015"/>
-    <s v="23 million"/>
+    <x v="38"/>
     <x v="48"/>
   </r>
   <r>
-    <s v="The Shack"/>
+    <x v="95"/>
     <s v="William P. Young"/>
     <x v="0"/>
     <s v="2007"/>
-    <s v="22.5 million"/>
+    <x v="39"/>
     <x v="11"/>
   </r>
   <r>
-    <s v="Uncle Styopa"/>
+    <x v="96"/>
     <s v="Sergey Mikhalkov"/>
     <x v="9"/>
     <s v="1936"/>
-    <s v="21 million"/>
+    <x v="40"/>
     <x v="25"/>
   </r>
   <r>
-    <s v="The Godfather"/>
+    <x v="97"/>
     <s v="Mario Puzo"/>
     <x v="0"/>
     <s v="1969"/>
-    <s v="21 million"/>
+    <x v="40"/>
     <x v="49"/>
   </r>
   <r>
-    <s v="Love Story"/>
+    <x v="98"/>
     <s v="Erich Segal"/>
     <x v="0"/>
     <s v="1970"/>
-    <s v="21 million"/>
+    <x v="40"/>
     <x v="50"/>
   </r>
   <r>
-    <s v="Catching Fire"/>
+    <x v="99"/>
     <s v="Suzanne Collins"/>
     <x v="0"/>
     <s v="2009"/>
-    <s v="21 million"/>
+    <x v="40"/>
     <x v="51"/>
   </r>
   <r>
-    <s v="Mockingjay"/>
+    <x v="100"/>
     <s v="Suzanne Collins"/>
     <x v="0"/>
     <s v="2010"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="52"/>
   </r>
   <r>
-    <s v="Kitchen"/>
+    <x v="101"/>
     <s v="Banana Yoshimoto"/>
     <x v="12"/>
     <s v="1988"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="53"/>
   </r>
   <r>
-    <s v="Andromeda Nebula"/>
+    <x v="102"/>
     <s v="Ivan Yefremov"/>
     <x v="9"/>
     <s v="1957"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="54"/>
   </r>
   <r>
-    <s v="Gone Girl"/>
+    <x v="103"/>
     <s v="Gillian Flynn"/>
     <x v="0"/>
     <s v="2012"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="55"/>
   </r>
   <r>
-    <s v="The Bermuda Triangle"/>
+    <x v="104"/>
     <s v="Charles Berlitz"/>
     <x v="0"/>
     <s v="1974"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="55"/>
   </r>
   <r>
-    <s v="Things Fall Apart"/>
+    <x v="105"/>
     <s v="Chinua Achebe"/>
     <x v="0"/>
     <s v="1958"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="11"/>
   </r>
   <r>
-    <s v="Wolf Totem"/>
+    <x v="106"/>
     <s v="Jiang Rong"/>
     <x v="2"/>
     <s v="2004"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="56"/>
   </r>
   <r>
-    <s v="The Happy Hooker: My Own Story"/>
+    <x v="107"/>
     <s v="Xaviera Hollander"/>
     <x v="0"/>
     <s v="1971"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="57"/>
   </r>
   <r>
-    <s v="Jaws"/>
+    <x v="108"/>
     <s v="Peter Benchley"/>
     <x v="0"/>
     <s v="1974"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="48"/>
   </r>
   <r>
-    <s v="Love You Forever"/>
+    <x v="109"/>
     <s v="Robert Munsch"/>
     <x v="0"/>
     <s v="1986"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="58"/>
   </r>
   <r>
-    <s v="The Women's Room"/>
+    <x v="110"/>
     <s v="Marilyn French"/>
     <x v="0"/>
     <s v="1977"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="59"/>
   </r>
   <r>
-    <s v="What to Expect When You're Expecting"/>
+    <x v="111"/>
     <s v="Arlene Eisenberg and Heidi Murkoff"/>
     <x v="0"/>
     <s v="1984"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="60"/>
   </r>
   <r>
-    <s v="Adventures of Huckleberry Finn"/>
+    <x v="112"/>
     <s v="Mark Twain"/>
     <x v="0"/>
     <s v="1885"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="61"/>
   </r>
   <r>
-    <s v="The Secret Diary of Adrian Mole, Aged 13¾"/>
+    <x v="113"/>
     <s v="Sue Townsend"/>
     <x v="0"/>
     <s v="1982"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="62"/>
   </r>
   <r>
-    <s v="Pride and Prejudice"/>
+    <x v="114"/>
     <s v="Jane Austen"/>
     <x v="0"/>
     <s v="1813"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="63"/>
   </r>
   <r>
-    <s v="Kon-Tiki: Across the Pacific in a Raft"/>
+    <x v="115"/>
     <s v="Thor Heyerdahl"/>
     <x v="8"/>
     <s v="1950"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="64"/>
   </r>
   <r>
-    <s v="The Good Soldier vejk"/>
+    <x v="116"/>
     <s v="Jaroslav Haek"/>
     <x v="13"/>
     <s v="1923"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="65"/>
   </r>
   <r>
-    <s v="Where the Wild Things Are"/>
+    <x v="117"/>
     <s v="Maurice Sendak"/>
     <x v="0"/>
     <s v="1963"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="66"/>
   </r>
   <r>
-    <s v="The Power of Positive Thinking"/>
+    <x v="118"/>
     <s v="Norman Vincent Peale"/>
     <x v="0"/>
     <s v="1952"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="35"/>
   </r>
   <r>
-    <s v="The Secret"/>
+    <x v="119"/>
     <s v="Rhonda Byrne"/>
     <x v="0"/>
     <s v="2006"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="35"/>
   </r>
   <r>
-    <s v="Fear of Flying"/>
+    <x v="120"/>
     <s v="Erica Jong"/>
     <x v="0"/>
     <s v="1973"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="67"/>
   </r>
   <r>
-    <s v="Dune"/>
+    <x v="121"/>
     <s v="Frank Herbert"/>
     <x v="0"/>
     <s v="1965"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="54"/>
   </r>
   <r>
-    <s v="Charlie and the Chocolate Factory"/>
+    <x v="122"/>
     <s v="Roald Dahl"/>
     <x v="0"/>
     <s v="1964"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="68"/>
   </r>
   <r>
-    <s v="The Naked Ape"/>
+    <x v="123"/>
     <s v="Desmond Morris"/>
     <x v="0"/>
     <s v="1968"/>
-    <s v="20 million"/>
+    <x v="41"/>
     <x v="69"/>
   </r>
   <r>
-    <s v="Momo"/>
+    <x v="124"/>
     <s v="Michael Ende"/>
     <x v="6"/>
     <s v="1973"/>
-    <s v="13 million"/>
+    <x v="18"/>
     <x v="15"/>
   </r>
   <r>
-    <s v="Peyton Place"/>
+    <x v="125"/>
     <s v="Grace Metalious"/>
     <x v="0"/>
     <s v="1956"/>
-    <s v="12.1 million"/>
+    <x v="42"/>
     <x v="15"/>
   </r>
   <r>
-    <s v="The Giver"/>
+    <x v="126"/>
     <s v="Lois Lowry"/>
     <x v="0"/>
     <s v="1993"/>
-    <s v="12 million"/>
+    <x v="43"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="Me Before You"/>
+    <x v="127"/>
     <s v="Jojo Moyes"/>
     <x v="0"/>
     <s v="2012"/>
-    <s v="12 million"/>
+    <x v="43"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="Norwegian Wood"/>
+    <x v="128"/>
     <s v="Haruki Murakami"/>
     <x v="12"/>
     <s v="1987"/>
-    <s v="12 million"/>
+    <x v="43"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="The Plague"/>
+    <x v="129"/>
     <s v="Albert Camus"/>
     <x v="1"/>
     <s v="1947"/>
-    <s v="12 million"/>
+    <x v="43"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="No Longer Human"/>
+    <x v="130"/>
     <s v="Osamu Dazai"/>
     <x v="12"/>
     <s v="1948"/>
-    <s v="12 million"/>
+    <x v="43"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="Man's Search for Meaning"/>
+    <x v="131"/>
     <s v="Viktor Frankl"/>
     <x v="6"/>
     <s v="1946"/>
-    <s v="12 million"/>
+    <x v="43"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="The Divine Comedy"/>
+    <x v="132"/>
     <s v="Dante Alighieri"/>
     <x v="7"/>
     <s v="1304"/>
-    <s v="1112 million"/>
+    <x v="44"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="The Prophet"/>
+    <x v="133"/>
     <s v="Kahlil Gibran"/>
     <x v="0"/>
     <s v="1923"/>
-    <s v="11 million"/>
+    <x v="45"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="The Boy in the Striped Pyjamas"/>
+    <x v="134"/>
     <s v="John Boyne"/>
     <x v="0"/>
     <s v="2006"/>
-    <s v="11 million"/>
+    <x v="45"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="The Exorcist"/>
+    <x v="135"/>
     <s v="William Peter Blatty"/>
     <x v="0"/>
     <s v="1971"/>
-    <s v="11 million"/>
+    <x v="45"/>
     <x v="71"/>
   </r>
   <r>
-    <s v="The Gruffalo"/>
+    <x v="136"/>
     <s v="Julia Donaldson"/>
     <x v="0"/>
     <s v="1999"/>
-    <s v="10.5 million"/>
+    <x v="46"/>
     <x v="71"/>
   </r>
   <r>
-    <s v="Fifty Shades Darker"/>
+    <x v="137"/>
     <s v="E. L. James"/>
     <x v="0"/>
     <s v="2012"/>
-    <s v="10.4 million"/>
+    <x v="47"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Tobacco Road"/>
+    <x v="138"/>
     <s v="Erskine Caldwell"/>
     <x v="0"/>
     <s v="1932"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Ronia, the Robber's Daughter"/>
+    <x v="139"/>
     <s v="Astrid Lindgren"/>
     <x v="11"/>
     <n v="1981"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Cat in the Hat"/>
+    <x v="140"/>
     <s v="Dr. Seuss"/>
     <x v="0"/>
     <s v="1957"/>
-    <s v="10.5 million"/>
+    <x v="46"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Diana: Her True Story"/>
+    <x v="141"/>
     <s v="Andrew Morton"/>
     <x v="0"/>
     <s v="1992"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Help"/>
+    <x v="142"/>
     <s v="Kathryn Stockett"/>
     <x v="0"/>
     <s v="2009"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Catch-22"/>
+    <x v="143"/>
     <s v="Joseph Heller"/>
     <x v="0"/>
     <s v="1961"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Stranger"/>
+    <x v="144"/>
     <s v="Albert Camus"/>
     <x v="1"/>
     <s v="1942"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Eye of the Needle"/>
+    <x v="145"/>
     <s v="Ken Follett"/>
     <x v="0"/>
     <s v="1978"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Lovely Bones"/>
+    <x v="146"/>
     <s v="Alice Sebold"/>
     <x v="0"/>
     <s v="2002"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Wild Swans"/>
+    <x v="147"/>
     <s v="Jung Chang"/>
     <x v="0"/>
     <s v="1992"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Santa Evita"/>
+    <x v="148"/>
     <s v="Tomás Eloy Martínez"/>
     <x v="5"/>
     <s v="1995"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Night"/>
+    <x v="149"/>
     <s v="Elie Wiesel"/>
     <x v="14"/>
     <s v="1958"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Confucius from the Heart"/>
+    <x v="150"/>
     <s v="Yu Dan"/>
     <x v="2"/>
     <s v="2006"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Total Woman"/>
+    <x v="151"/>
     <s v="Marabel Morgan"/>
     <x v="0"/>
     <s v="1974"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Knowledge-value Revolution"/>
+    <x v="152"/>
     <s v="Taichi Sakaiya"/>
     <x v="12"/>
     <s v="1985"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Problems in China's Socialist Economy"/>
+    <x v="153"/>
     <s v="Xue Muqiao"/>
     <x v="2"/>
     <s v="1979"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="What Color Is Your Parachute?"/>
+    <x v="154"/>
     <s v="Richard Nelson Bolles"/>
     <x v="0"/>
     <s v="1970"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Dukan Diet"/>
+    <x v="155"/>
     <s v="Pierre Dukan"/>
     <x v="1"/>
     <s v="2000"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Joy of Sex"/>
+    <x v="156"/>
     <s v="Alex Comfort"/>
     <x v="0"/>
     <s v="1972"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Gospel According to Peanuts"/>
+    <x v="157"/>
     <s v="Robert L. Short"/>
     <x v="0"/>
     <s v="1965"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Subtle Art of Not Giving a Fuck"/>
+    <x v="158"/>
     <s v="Mark Manson"/>
     <x v="0"/>
     <s v="2016"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Life of Pi"/>
+    <x v="159"/>
     <s v="Yann Martel"/>
     <x v="0"/>
     <s v="2001"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Front Runner"/>
+    <x v="160"/>
     <s v="Patricia Nell Warren"/>
     <x v="0"/>
     <s v="1974"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Goal"/>
+    <x v="161"/>
     <s v="Eliyahu M. Goldratt"/>
     <x v="0"/>
     <n v="1984"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Fahrenheit 451"/>
+    <x v="162"/>
     <s v="Ray Bradbury"/>
     <x v="0"/>
     <n v="1953"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="70"/>
   </r>
   <r>
-    <s v="Angela's Ashes"/>
+    <x v="163"/>
     <s v="Frank McCourt"/>
     <x v="0"/>
     <n v="1996"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="The Story of My Experiments with Truth"/>
+    <x v="164"/>
     <s v="Mohandas Karamchand Gandhi"/>
     <x v="15"/>
     <n v="1929"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Bridget Jones's Diary"/>
+    <x v="165"/>
     <s v="Helen Fielding"/>
     <x v="0"/>
     <s v="1996"/>
-    <s v="10 million"/>
+    <x v="48"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="World Almanac"/>
+    <x v="166"/>
     <s v="Various authors"/>
     <x v="0"/>
     <n v="1868"/>
-    <s v="82 million"/>
+    <x v="49"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Betty Crocker Cookbook"/>
+    <x v="167"/>
     <s v="General Mills staff"/>
     <x v="0"/>
     <n v="1950"/>
-    <s v="75 million"/>
+    <x v="50"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Tung Shing"/>
+    <x v="168"/>
     <s v="Choi Park Lai's family, among others"/>
     <x v="2"/>
     <n v="1891"/>
-    <s v="&gt;70 million"/>
+    <x v="51"/>
     <x v="22"/>
   </r>
   <r>
-    <s v="Merriam-Webster's Collegiate Dictionary"/>
+    <x v="169"/>
     <s v="Merriam-Webster"/>
     <x v="0"/>
     <s v="1898"/>
-    <s v="55 million"/>
+    <x v="52"/>
     <x v="22"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF4B4A71-DEED-4CC9-A8A4-15EFBED8109B}" name="PivotTable5" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA0E6B59-6726-46BE-BFE0-B879A351483D}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L3:M174" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="171">
+        <item x="85"/>
+        <item x="59"/>
+        <item x="0"/>
+        <item x="52"/>
+        <item x="112"/>
+        <item x="36"/>
+        <item x="3"/>
+        <item x="102"/>
+        <item x="163"/>
+        <item x="64"/>
+        <item x="22"/>
+        <item x="47"/>
+        <item x="167"/>
+        <item x="23"/>
+        <item x="165"/>
+        <item x="143"/>
+        <item x="99"/>
+        <item x="122"/>
+        <item x="28"/>
+        <item x="150"/>
+        <item x="62"/>
+        <item x="141"/>
+        <item x="4"/>
+        <item x="121"/>
+        <item x="145"/>
+        <item x="162"/>
+        <item x="120"/>
+        <item x="137"/>
+        <item x="37"/>
+        <item x="61"/>
+        <item x="51"/>
+        <item x="50"/>
+        <item x="103"/>
+        <item x="76"/>
+        <item x="34"/>
+        <item x="39"/>
+        <item x="9"/>
+        <item x="14"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="10"/>
+        <item x="20"/>
+        <item x="66"/>
+        <item x="74"/>
+        <item x="46"/>
+        <item x="82"/>
+        <item x="108"/>
+        <item x="57"/>
+        <item x="65"/>
+        <item x="101"/>
+        <item x="152"/>
+        <item x="115"/>
+        <item x="55"/>
+        <item x="159"/>
+        <item x="19"/>
+        <item x="53"/>
+        <item x="98"/>
+        <item x="109"/>
+        <item x="87"/>
+        <item x="131"/>
+        <item x="31"/>
+        <item x="127"/>
+        <item x="169"/>
+        <item x="100"/>
+        <item x="124"/>
+        <item x="149"/>
+        <item x="130"/>
+        <item x="128"/>
+        <item x="18"/>
+        <item x="86"/>
+        <item x="43"/>
+        <item x="125"/>
+        <item x="114"/>
+        <item x="153"/>
+        <item x="77"/>
+        <item x="139"/>
+        <item x="148"/>
+        <item x="40"/>
+        <item x="6"/>
+        <item x="63"/>
+        <item x="89"/>
+        <item x="68"/>
+        <item x="15"/>
+        <item x="104"/>
+        <item x="32"/>
+        <item x="134"/>
+        <item x="17"/>
+        <item x="140"/>
+        <item x="16"/>
+        <item x="92"/>
+        <item x="21"/>
+        <item x="8"/>
+        <item x="69"/>
+        <item x="132"/>
+        <item x="155"/>
+        <item x="25"/>
+        <item x="135"/>
+        <item x="93"/>
+        <item x="160"/>
+        <item x="29"/>
+        <item x="94"/>
+        <item x="79"/>
+        <item x="126"/>
+        <item x="161"/>
+        <item x="97"/>
+        <item x="116"/>
+        <item x="157"/>
+        <item x="44"/>
+        <item x="75"/>
+        <item x="136"/>
+        <item x="107"/>
+        <item x="142"/>
+        <item x="48"/>
+        <item x="27"/>
+        <item x="5"/>
+        <item x="33"/>
+        <item x="81"/>
+        <item x="156"/>
+        <item x="72"/>
+        <item x="1"/>
+        <item x="80"/>
+        <item x="146"/>
+        <item x="123"/>
+        <item x="24"/>
+        <item x="35"/>
+        <item x="54"/>
+        <item x="38"/>
+        <item x="42"/>
+        <item x="129"/>
+        <item x="41"/>
+        <item x="118"/>
+        <item x="133"/>
+        <item x="78"/>
+        <item x="119"/>
+        <item x="113"/>
+        <item x="95"/>
+        <item x="45"/>
+        <item x="164"/>
+        <item x="144"/>
+        <item x="158"/>
+        <item x="56"/>
+        <item x="71"/>
+        <item x="151"/>
+        <item x="58"/>
+        <item x="88"/>
+        <item x="110"/>
+        <item x="83"/>
+        <item x="105"/>
+        <item x="60"/>
+        <item x="138"/>
+        <item x="90"/>
+        <item x="49"/>
+        <item x="168"/>
+        <item x="96"/>
+        <item x="73"/>
+        <item x="7"/>
+        <item x="91"/>
+        <item x="67"/>
+        <item x="26"/>
+        <item x="154"/>
+        <item x="111"/>
+        <item x="30"/>
+        <item x="117"/>
+        <item x="84"/>
+        <item x="147"/>
+        <item x="106"/>
+        <item x="166"/>
+        <item x="70"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="54">
+        <item x="0"/>
+        <item x="31"/>
+        <item x="51"/>
+        <item x="5"/>
+        <item x="48"/>
+        <item x="47"/>
+        <item x="46"/>
+        <item x="3"/>
+        <item x="45"/>
+        <item x="44"/>
+        <item x="43"/>
+        <item x="42"/>
+        <item x="2"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="15"/>
+        <item x="14"/>
+        <item x="13"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="41"/>
+        <item x="1"/>
+        <item x="40"/>
+        <item x="39"/>
+        <item x="38"/>
+        <item x="37"/>
+        <item x="36"/>
+        <item x="35"/>
+        <item x="34"/>
+        <item x="33"/>
+        <item x="32"/>
+        <item x="30"/>
+        <item x="29"/>
+        <item x="28"/>
+        <item x="27"/>
+        <item x="26"/>
+        <item x="25"/>
+        <item x="24"/>
+        <item x="23"/>
+        <item x="22"/>
+        <item x="21"/>
+        <item x="20"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="52"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="50"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="49"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="171">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="63"/>
+    </i>
+    <i>
+      <x v="64"/>
+    </i>
+    <i>
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="66"/>
+    </i>
+    <i>
+      <x v="67"/>
+    </i>
+    <i>
+      <x v="68"/>
+    </i>
+    <i>
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="70"/>
+    </i>
+    <i>
+      <x v="71"/>
+    </i>
+    <i>
+      <x v="72"/>
+    </i>
+    <i>
+      <x v="73"/>
+    </i>
+    <i>
+      <x v="74"/>
+    </i>
+    <i>
+      <x v="75"/>
+    </i>
+    <i>
+      <x v="76"/>
+    </i>
+    <i>
+      <x v="77"/>
+    </i>
+    <i>
+      <x v="78"/>
+    </i>
+    <i>
+      <x v="79"/>
+    </i>
+    <i>
+      <x v="80"/>
+    </i>
+    <i>
+      <x v="81"/>
+    </i>
+    <i>
+      <x v="82"/>
+    </i>
+    <i>
+      <x v="83"/>
+    </i>
+    <i>
+      <x v="84"/>
+    </i>
+    <i>
+      <x v="85"/>
+    </i>
+    <i>
+      <x v="86"/>
+    </i>
+    <i>
+      <x v="87"/>
+    </i>
+    <i>
+      <x v="88"/>
+    </i>
+    <i>
+      <x v="89"/>
+    </i>
+    <i>
+      <x v="90"/>
+    </i>
+    <i>
+      <x v="91"/>
+    </i>
+    <i>
+      <x v="92"/>
+    </i>
+    <i>
+      <x v="93"/>
+    </i>
+    <i>
+      <x v="94"/>
+    </i>
+    <i>
+      <x v="95"/>
+    </i>
+    <i>
+      <x v="96"/>
+    </i>
+    <i>
+      <x v="97"/>
+    </i>
+    <i>
+      <x v="98"/>
+    </i>
+    <i>
+      <x v="99"/>
+    </i>
+    <i>
+      <x v="100"/>
+    </i>
+    <i>
+      <x v="101"/>
+    </i>
+    <i>
+      <x v="102"/>
+    </i>
+    <i>
+      <x v="103"/>
+    </i>
+    <i>
+      <x v="104"/>
+    </i>
+    <i>
+      <x v="105"/>
+    </i>
+    <i>
+      <x v="106"/>
+    </i>
+    <i>
+      <x v="107"/>
+    </i>
+    <i>
+      <x v="108"/>
+    </i>
+    <i>
+      <x v="109"/>
+    </i>
+    <i>
+      <x v="110"/>
+    </i>
+    <i>
+      <x v="111"/>
+    </i>
+    <i>
+      <x v="112"/>
+    </i>
+    <i>
+      <x v="113"/>
+    </i>
+    <i>
+      <x v="114"/>
+    </i>
+    <i>
+      <x v="115"/>
+    </i>
+    <i>
+      <x v="116"/>
+    </i>
+    <i>
+      <x v="117"/>
+    </i>
+    <i>
+      <x v="118"/>
+    </i>
+    <i>
+      <x v="119"/>
+    </i>
+    <i>
+      <x v="120"/>
+    </i>
+    <i>
+      <x v="121"/>
+    </i>
+    <i>
+      <x v="122"/>
+    </i>
+    <i>
+      <x v="123"/>
+    </i>
+    <i>
+      <x v="124"/>
+    </i>
+    <i>
+      <x v="125"/>
+    </i>
+    <i>
+      <x v="126"/>
+    </i>
+    <i>
+      <x v="127"/>
+    </i>
+    <i>
+      <x v="128"/>
+    </i>
+    <i>
+      <x v="129"/>
+    </i>
+    <i>
+      <x v="130"/>
+    </i>
+    <i>
+      <x v="131"/>
+    </i>
+    <i>
+      <x v="132"/>
+    </i>
+    <i>
+      <x v="133"/>
+    </i>
+    <i>
+      <x v="134"/>
+    </i>
+    <i>
+      <x v="135"/>
+    </i>
+    <i>
+      <x v="136"/>
+    </i>
+    <i>
+      <x v="137"/>
+    </i>
+    <i>
+      <x v="138"/>
+    </i>
+    <i>
+      <x v="139"/>
+    </i>
+    <i>
+      <x v="140"/>
+    </i>
+    <i>
+      <x v="141"/>
+    </i>
+    <i>
+      <x v="142"/>
+    </i>
+    <i>
+      <x v="143"/>
+    </i>
+    <i>
+      <x v="144"/>
+    </i>
+    <i>
+      <x v="145"/>
+    </i>
+    <i>
+      <x v="146"/>
+    </i>
+    <i>
+      <x v="147"/>
+    </i>
+    <i>
+      <x v="148"/>
+    </i>
+    <i>
+      <x v="149"/>
+    </i>
+    <i>
+      <x v="150"/>
+    </i>
+    <i>
+      <x v="151"/>
+    </i>
+    <i>
+      <x v="152"/>
+    </i>
+    <i>
+      <x v="153"/>
+    </i>
+    <i>
+      <x v="154"/>
+    </i>
+    <i>
+      <x v="155"/>
+    </i>
+    <i>
+      <x v="156"/>
+    </i>
+    <i>
+      <x v="157"/>
+    </i>
+    <i>
+      <x v="158"/>
+    </i>
+    <i>
+      <x v="159"/>
+    </i>
+    <i>
+      <x v="160"/>
+    </i>
+    <i>
+      <x v="161"/>
+    </i>
+    <i>
+      <x v="162"/>
+    </i>
+    <i>
+      <x v="163"/>
+    </i>
+    <i>
+      <x v="164"/>
+    </i>
+    <i>
+      <x v="165"/>
+    </i>
+    <i>
+      <x v="166"/>
+    </i>
+    <i>
+      <x v="167"/>
+    </i>
+    <i>
+      <x v="168"/>
+    </i>
+    <i>
+      <x v="169"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Approximate sales" fld="4" baseField="0" baseItem="11"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF4B4A71-DEED-4CC9-A8A4-15EFBED8109B}" name="PivotTable5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="9">
   <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -4518,7 +5529,7 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="3" xr16:uid="{A6433183-E3A3-4D43-B2D2-4031B7ECA212}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="17">
+  <queryTableRefresh nextId="18">
     <queryTableFields count="6">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
@@ -4812,7 +5823,7 @@
   <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F166" sqref="F166"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8254,106 +9265,1475 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B71716-EBB4-445B-96B7-6B5D8C4D835A}">
+  <dimension ref="A3:M174"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B71716-EBB4-445B-96B7-6B5D8C4D835A}">
-  <dimension ref="A3:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="34" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="45" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="65" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L3" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="M3" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>188</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>246</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L7" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L8" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>3</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L12" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L27" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L28" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L31" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L33" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L34" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L35" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="M35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L36" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="M36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L37" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L39" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L48" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="M48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L49" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="M49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L50" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L51" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L52" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="M52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L53" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="M53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L54" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L55" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="M55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L56" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="M56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L57" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="M57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L58" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L59" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="M59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L60" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="M61" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L62" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="M62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L63" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="M63" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L64" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="M64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L65" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="M65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L67" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="M67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L68" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="M68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L69" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="M69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L70" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="M70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L71" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="M71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L72" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="M72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L73" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="M73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L74" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="M74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L75" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="M75" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L76" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="M76" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L77" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="M77" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L78" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="M78" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L79" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="M79" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L80" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M80" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L81" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="M81" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L82" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="M82" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L83" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M83" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L84" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M84" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L85" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="M85" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L86" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M86" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L87" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="M87" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L88" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="M88" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L89" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="M89" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L90" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M90" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L91" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="M91" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L92" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M92" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L93" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="M93" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L94" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M94" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L95" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M95" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L96" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M96" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L97" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M97" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L98" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="M98" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L99" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="M99" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L100" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="M100" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L101" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M101" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L102" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="M102" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L103" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="M103" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L104" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="M104" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L105" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M105" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L106" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M106" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L107" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="M107" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L108" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="M108" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L109" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="M109" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L110" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="M110" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L111" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="M111" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L112" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="M112" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L113" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M113" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L114" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="M114" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L115" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="M115" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L116" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="M116" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L117" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="M117" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L118" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M118" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L119" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M119" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L120" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M120" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L121" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M121" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L122" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="M122" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L123" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="M123" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L124" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="M124" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L125" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="M125" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L126" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M126" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L127" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="M127" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L128" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="M128" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L129" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="M129" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L130" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="M130" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L131" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M131" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L132" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M132" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L133" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M133" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L134" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="M134" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L135" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M135" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L136" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="M136" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L137" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="M137" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L138" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="M138" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L139" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="M139" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L140" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="M140" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L141" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="M141" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L142" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="M142" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L143" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="M143" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L144" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="M144" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L145" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="M145" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L146" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M146" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L147" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M147" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L148" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="M148" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L149" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M149" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L150" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="M150" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L151" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="M151" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L152" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="M152" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L153" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="M153" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L154" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M154" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L155" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="M155" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L156" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="M156" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L157" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M157" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L158" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="M158" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L159" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="M159" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L160" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="M160" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L161" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="M161" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L162" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="M162" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L163" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="M163" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L164" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M164" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L165" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="M165" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L166" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="M166" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L167" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M167" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L168" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="M168" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L169" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="M169" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L170" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="M170" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L171" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="M171" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L172" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="M172" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L173" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="M173" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L174" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="M174" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>